<commit_message>
agregando frases claves para identificar preguntas administrativas (las que no van a ir a embeddings) y relizando el análisis de las preguntas y sus respuestas
</commit_message>
<xml_diff>
--- a/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
+++ b/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\python_con_json\obtener_preguntas_y_respuestas\docs\Analisis_de_resultados\analisis_22_05_25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E2B780-0119-4235-AD58-AA1B2C178DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E917F-52B5-49AC-A2BC-23DC7FB0D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="38">
   <si>
     <t>pregunta</t>
   </si>
@@ -318,32 +318,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">En el JSON 1 analicé 63 preguntas, me dio 84% respondidas. Como el margen de error es ±9.05%, el valor real podría estar entre 75,08 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% y 93,05%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>n</t>
     </r>
     <r>
@@ -382,8 +356,14 @@
     <t>respuestas extras</t>
   </si>
   <si>
+    <t>En el JSON 1 analicé 63 preguntas, me dio 90,48% respondidas. Como el margen de error es ±7.25%, el valor real podría estar entre 83,23 % y 97,73%.</t>
+  </si>
+  <si>
+    <t>En el JSON 1 analicé 51 preguntas, me dio 92% respondidas. Como el margen de error es ±7.38%, el valor real podría estar entre 84,62 % y 99,38%.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">En el JSON 1 analicé 63 preguntas, me dio 90,48% respondidas. Como el margen de error es ±7.25%, el valor real podría estar entre 83,23 </t>
+      <t xml:space="preserve">En el JSON 1 analicé 46 preguntas, me dio 84% respondidas. Como el margen de error es ±9.05%, el valor real podría estar entre 75,08 </t>
     </r>
     <r>
       <rPr>
@@ -394,7 +374,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>% y 97,73%</t>
+      <t>% y 93,05%</t>
     </r>
     <r>
       <rPr>
@@ -476,17 +456,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,7 +881,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -915,13 +894,12 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="6" width="13.88671875" customWidth="1"/>
@@ -931,11 +909,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -947,10 +925,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -964,19 +942,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
@@ -997,19 +975,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G64" si="0">IF(B3="si",1,0)</f>
@@ -1025,24 +1003,24 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4">
         <f t="shared" ref="A4:A64" si="3">A3+3</f>
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -1063,19 +1041,19 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -1091,18 +1069,18 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -1118,18 +1096,18 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1145,18 +1123,18 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1172,18 +1150,18 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -1199,18 +1177,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -1226,18 +1204,18 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -1253,18 +1231,18 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -1285,13 +1263,13 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -1312,13 +1290,13 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -1339,13 +1317,13 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1361,21 +1339,21 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -1391,21 +1369,21 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -1426,13 +1404,13 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -1448,18 +1426,18 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -1475,21 +1453,21 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -1505,18 +1483,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -1537,298 +1515,298 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <f t="shared" si="3"/>
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <f t="shared" si="3"/>
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <f t="shared" si="3"/>
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <f t="shared" si="3"/>
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <f t="shared" si="3"/>
-        <v>82</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <f t="shared" si="3"/>
-        <v>85</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
-        <f t="shared" si="3"/>
-        <v>88</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32">
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -1844,18 +1822,18 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -1871,18 +1849,18 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34">
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
@@ -1898,18 +1876,18 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -1930,13 +1908,13 @@
         <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
@@ -1952,18 +1930,18 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37">
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
@@ -1979,18 +1957,18 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38">
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
@@ -2011,13 +1989,13 @@
         <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
@@ -2033,21 +2011,21 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="A40">
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
@@ -2068,13 +2046,13 @@
         <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
@@ -2095,13 +2073,13 @@
         <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
@@ -2117,18 +2095,18 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="6">
+      <c r="A43" s="5">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
@@ -2144,18 +2122,18 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44">
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
@@ -2171,18 +2149,18 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+      <c r="A45">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
@@ -2203,13 +2181,13 @@
         <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
@@ -2225,18 +2203,18 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+      <c r="A47">
         <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
@@ -2252,18 +2230,18 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="6">
+      <c r="A48" s="5">
         <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
@@ -2279,18 +2257,18 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="8">
+      <c r="A49" s="6">
         <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G49">
         <f t="shared" si="0"/>
@@ -2306,18 +2284,18 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+      <c r="A50">
         <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50">
         <f t="shared" si="0"/>
@@ -2333,18 +2311,18 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="5">
+      <c r="A51">
         <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G51">
         <f t="shared" si="0"/>
@@ -2365,13 +2343,13 @@
         <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G52">
         <f t="shared" si="0"/>
@@ -2392,13 +2370,13 @@
         <v>154</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G53">
         <f t="shared" si="0"/>
@@ -2414,18 +2392,18 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="5">
+      <c r="A54">
         <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G54">
         <f t="shared" si="0"/>
@@ -2441,18 +2419,18 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="5">
+      <c r="A55">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55">
         <f t="shared" si="0"/>
@@ -2468,21 +2446,21 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="5">
+      <c r="A56">
         <f t="shared" si="3"/>
         <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G56">
         <f t="shared" si="0"/>
@@ -2498,18 +2476,18 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="5">
+      <c r="A57">
         <f t="shared" si="3"/>
         <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G57">
         <f t="shared" si="0"/>
@@ -2525,18 +2503,18 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="6">
+      <c r="A58" s="5">
         <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G58">
         <f t="shared" si="0"/>
@@ -2550,23 +2528,23 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J58" s="7" t="s">
-        <v>34</v>
+      <c r="J58" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="5">
+      <c r="A59">
         <f t="shared" si="3"/>
         <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G59">
         <f t="shared" si="0"/>
@@ -2587,13 +2565,13 @@
         <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G60">
         <f t="shared" si="0"/>
@@ -2609,18 +2587,18 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="5">
+      <c r="A61">
         <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G61">
         <f t="shared" si="0"/>
@@ -2636,18 +2614,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="5">
+      <c r="A62">
         <f t="shared" si="3"/>
         <v>181</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G62">
         <f t="shared" si="0"/>
@@ -2663,18 +2641,18 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="5">
+      <c r="A63">
         <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G63">
         <f t="shared" si="0"/>
@@ -2690,18 +2668,18 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="5">
+      <c r="A64">
         <f t="shared" si="3"/>
         <v>187</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G64">
         <f t="shared" si="0"/>
@@ -2717,7 +2695,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+      <c r="A65" t="s">
         <v>6</v>
       </c>
       <c r="G65">
@@ -2734,13 +2712,13 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="5">
+      <c r="A66">
         <f>COUNT(A2:A64)</f>
         <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+      <c r="A69" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="2">
@@ -2749,8 +2727,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>35</v>
+      <c r="A70" t="s">
+        <v>34</v>
       </c>
       <c r="C70" s="2">
         <f>I65/A66</f>
@@ -2758,12 +2736,12 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+      <c r="A72" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+      <c r="A73" t="s">
         <v>19</v>
       </c>
       <c r="C73" s="2">
@@ -2772,7 +2750,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+      <c r="A74" t="s">
         <v>23</v>
       </c>
       <c r="C74">
@@ -2780,16 +2758,16 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
+      <c r="A75" t="s">
         <v>24</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="7">
         <f>C69</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
+      <c r="A76" t="s">
         <v>25</v>
       </c>
       <c r="C76">
@@ -2798,8 +2776,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
-        <v>36</v>
+      <c r="A79" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2816,14 +2794,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492E6E18-1ECC-4D69-978F-0D695792FF82}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="6" width="13.88671875" customWidth="1"/>
@@ -2833,11 +2810,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2849,10 +2826,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -2862,20 +2839,20 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
@@ -2891,21 +2868,21 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3">
         <f>A2+3</f>
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:I52" si="0">IF(B3="si",1,0)</f>
@@ -2921,18 +2898,18 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4">
         <f t="shared" ref="A4:A52" si="1">A3+3</f>
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2948,21 +2925,21 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -2978,21 +2955,21 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -3008,18 +2985,18 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -3035,21 +3012,21 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -3065,18 +3042,18 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -3092,18 +3069,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -3119,18 +3096,18 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -3146,18 +3123,18 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -3173,18 +3150,18 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -3205,13 +3182,13 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -3227,18 +3204,18 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -3254,18 +3231,18 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -3286,13 +3263,13 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -3308,18 +3285,18 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -3335,53 +3312,86 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
@@ -3389,49 +3399,82 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
@@ -3439,17 +3482,26 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
@@ -3457,39 +3509,57 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -3497,53 +3567,86 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="A28">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
@@ -3551,17 +3654,26 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
@@ -3569,53 +3681,80 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
@@ -3623,17 +3762,26 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
@@ -3641,13 +3789,22 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
@@ -3655,21 +3812,33 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
@@ -3677,31 +3846,52 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="A39">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
       <c r="G39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
@@ -3709,93 +3899,141 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="A40">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
       <c r="G40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+      <c r="A41">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
       <c r="G41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="A42">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" t="s">
+        <v>30</v>
+      </c>
       <c r="G42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+      <c r="A43">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
       <c r="G43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
       <c r="G44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
@@ -3803,35 +4041,53 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+      <c r="A45">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
       <c r="G45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+      <c r="A46">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
       <c r="G46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
@@ -3839,17 +4095,26 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+      <c r="A47">
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
@@ -3857,17 +4122,26 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+      <c r="A48">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
       <c r="G48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
@@ -3875,122 +4149,175 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+      <c r="A49">
         <f t="shared" si="1"/>
         <v>142</v>
       </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
       <c r="G49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+      <c r="A50">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
       <c r="G50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="5">
+      <c r="A51">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
       <c r="G51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="5">
+      <c r="A52">
         <f t="shared" si="1"/>
         <v>151</v>
       </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
       <c r="G52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <f>SUM(G2:G52)</f>
+        <v>51</v>
+      </c>
+      <c r="H53">
+        <f>SUM(H2:H52)</f>
+        <v>47</v>
+      </c>
+      <c r="I53">
+        <f>SUM(I2:I52)</f>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="5">
+      <c r="A55">
         <f>COUNT(A2:A52)</f>
         <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="A57" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="2">
-        <f>H54/A55</f>
-        <v>0</v>
+        <f>H53/A55</f>
+        <v>0.92156862745098034</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="A58" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="2">
-        <f>I54/A55</f>
-        <v>0</v>
+        <f>I53/A55</f>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+      <c r="A60" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
+      <c r="A61" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="2">
         <f>C62*(C63*(1-C63)/C64)^(1/2)</f>
-        <v>0</v>
+        <v>7.378697935622161E-2</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+      <c r="A62" t="s">
         <v>23</v>
       </c>
       <c r="C62">
@@ -3998,13 +4325,16 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+      <c r="A63" t="s">
         <v>24</v>
       </c>
-      <c r="C63" s="4"/>
+      <c r="C63" s="2">
+        <f>C57</f>
+        <v>0.92156862745098034</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="A64" t="s">
         <v>25</v>
       </c>
       <c r="C64">
@@ -4013,13 +4343,13 @@
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
-        <v>26</v>
+      <c r="A67" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F53 B2:B52" xr:uid="{120475DA-F9BD-4311-B8DC-0100D5893165}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B52 C2:F53" xr:uid="{120475DA-F9BD-4311-B8DC-0100D5893165}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4031,14 +4361,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1FF2E0-CBF5-4429-A8E7-8C52D40AA9F4}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A25" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="6" width="13.88671875" customWidth="1"/>
@@ -4048,11 +4377,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4064,10 +4393,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -4077,16 +4406,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>IF(C2="si",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <f>IF(D2="si",1,0)</f>
@@ -4094,17 +4435,26 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="1">
         <f>A2+3</f>
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
       <c r="G3">
         <f t="shared" ref="G3:I47" si="0">IF(B3="si",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
@@ -4112,71 +4462,107 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4">
         <f t="shared" ref="A4:A47" si="1">A3+3</f>
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -4184,35 +4570,56 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -4220,17 +4627,29 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
@@ -4238,10 +4657,25 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4252,93 +4686,147 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <f t="shared" si="1"/>
-        <v>31</v>
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
@@ -4346,17 +4834,29 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
@@ -4364,13 +4864,22 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
@@ -4378,35 +4887,56 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
@@ -4414,39 +4944,60 @@
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
@@ -4454,53 +5005,89 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
@@ -4508,53 +5095,86 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="A28">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
@@ -4562,17 +5182,26 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
@@ -4580,17 +5209,26 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
@@ -4598,10 +5236,19 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
       <c r="G31">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4612,39 +5259,60 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
@@ -4652,13 +5320,22 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
@@ -4666,21 +5343,33 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
@@ -4688,7 +5377,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
@@ -4706,7 +5395,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
@@ -4724,7 +5413,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
@@ -4742,7 +5431,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="A39">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
@@ -4760,7 +5449,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="A40">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
@@ -4778,7 +5467,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+      <c r="A41">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
@@ -4796,7 +5485,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="A42">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
@@ -4814,7 +5503,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+      <c r="A43">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
@@ -4832,7 +5521,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
@@ -4850,7 +5539,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+      <c r="A45">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
@@ -4868,7 +5557,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+      <c r="A46">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
@@ -4886,7 +5575,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+      <c r="A47">
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
@@ -4904,53 +5593,53 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" t="s">
         <v>6</v>
       </c>
       <c r="G48">
         <f>SUM(G2:G47)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H48">
         <f>SUM(H2:H47)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I48">
         <f>SUM(I2:I47)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+      <c r="A49">
         <f>COUNT(A2:A47)</f>
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="A51" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="2">
         <f>H48/A49</f>
-        <v>0</v>
+        <v>0.63043478260869568</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="2">
         <f>I48/A49</f>
-        <v>0</v>
+        <v>0.43478260869565216</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="A55" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="2">
@@ -4959,7 +5648,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+      <c r="A56" t="s">
         <v>23</v>
       </c>
       <c r="C56">
@@ -4967,13 +5656,13 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="A57" t="s">
         <v>24</v>
       </c>
       <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="A58" t="s">
         <v>25</v>
       </c>
       <c r="C58">
@@ -4982,8 +5671,8 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>26</v>
+      <c r="A61" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizando análisis de preguntas y respuestas generadas y agregando frases típicas de respuestas administrativas identificadas
</commit_message>
<xml_diff>
--- a/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
+++ b/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\python_con_json\obtener_preguntas_y_respuestas\docs\Analisis_de_resultados\analisis_22_05_25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E917F-52B5-49AC-A2BC-23DC7FB0D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29462C60-E9AA-4153-8B18-7752CF729782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="5" r:id="rId1"/>
+    <sheet name="Referencias" sheetId="5" r:id="rId1"/>
     <sheet name="JSON_1" sheetId="1" r:id="rId2"/>
     <sheet name="JSON_2" sheetId="6" r:id="rId3"/>
     <sheet name="JSON_3" sheetId="7" r:id="rId4"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="38">
   <si>
     <t>pregunta</t>
   </si>
@@ -71,74 +71,6 @@
     <t>Considerando  95%  de confianza ( en 95 de cada 100 veces el resultado real va a estar dentro de un cierto rango)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">El </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>95% de confianza</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> significa que si repitieras el estudio muchas veces, el resultado </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>real</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> estaría dentro de ese intervalo el </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>95% de las veces</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Nos dice cuántos datos caen dentro de cierta área bajo la curva normal.</t>
   </si>
   <si>
@@ -151,161 +83,16 @@
     <t>La distribución normal estándar es una curva que modela muchos fenómenos naturales (como alturas de personas, errores de medición, etc.).</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">La </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>media</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (también llamada promedio) es el valor central de un conjunto de datos. Se calcula sumando </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>todos los valores</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> y dividiéndolos por la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cantidad de elementos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Si los datos están muy dispersos, la desviación es alta. Si están agrupados cerca de la media, es baja.</t>
   </si>
   <si>
     <t>Z es el número de desviaciones estándar desde la media. Es la distancia que hay entre un valor y la media.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">La </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>desviación estándar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> mide </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cuánto varían los datos respecto a la media</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>ME = Z *   (( p  * (1 -p) ) / n)^(1/2)</t>
   </si>
   <si>
     <t>Margen de Error</t>
-  </si>
-  <si>
-    <r>
-      <t>Z = 1.96</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> para el 95% de confianza.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> es la proporción de éxito (ej. 0.84).</t>
-    </r>
   </si>
   <si>
     <t>Z</t>
@@ -315,21 +102,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <r>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> es el tamaño de la muestra (ej. 63 preguntas).</t>
-    </r>
   </si>
   <si>
     <t>¿es efectivamente pregunta?</t>
@@ -359,40 +131,35 @@
     <t>En el JSON 1 analicé 63 preguntas, me dio 90,48% respondidas. Como el margen de error es ±7.25%, el valor real podría estar entre 83,23 % y 97,73%.</t>
   </si>
   <si>
-    <t>En el JSON 1 analicé 51 preguntas, me dio 92% respondidas. Como el margen de error es ±7.38%, el valor real podría estar entre 84,62 % y 99,38%.</t>
+    <t>En el JSON 2 analicé 51 preguntas, me dio 92% respondidas. Como el margen de error es ±7.38%, el valor real podría estar entre 84,62 % y 99,38%.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">En el JSON 1 analicé 46 preguntas, me dio 84% respondidas. Como el margen de error es ±9.05%, el valor real podría estar entre 75,08 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>% y 93,05%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
+    <t>En el JSON 3 analicé 46 preguntas, me dio 85% respondidas. Como el margen de error es ±10.38%, el valor real podría estar entre 74,62 % y 95,38%.</t>
+  </si>
+  <si>
+    <t>El 95% de confianza significa que si repitieras el estudio muchas veces, el resultado real estaría dentro de ese intervalo el 95% de las veces.</t>
+  </si>
+  <si>
+    <t>La media (también llamada promedio) es el valor central de un conjunto de datos. Se calcula sumando todos los valores y dividiéndolos por la cantidad de elementos.</t>
+  </si>
+  <si>
+    <t>La desviación estándar mide cuánto varían los datos respecto a la media.</t>
+  </si>
+  <si>
+    <t>Z = 1.96 para el 95% de confianza.</t>
+  </si>
+  <si>
+    <t>p es la proporción de éxito (ej. 0.84).</t>
+  </si>
+  <si>
+    <t>n es el tamaño de la muestra (ej. 63 preguntas).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,14 +168,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -456,14 +215,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -803,85 +560,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AA836D-385C-4141-AF5A-AAFCA35CFBC3}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
+      <c r="A15" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
+      <c r="A16" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>26</v>
+      <c r="A17" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -925,10 +688,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -942,19 +705,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
@@ -975,19 +738,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G64" si="0">IF(B3="si",1,0)</f>
@@ -1008,19 +771,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -1041,19 +804,19 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -1074,13 +837,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -1101,13 +864,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1128,13 +891,13 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1155,13 +918,13 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -1182,13 +945,13 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -1209,13 +972,13 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -1236,13 +999,13 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -1263,13 +1026,13 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -1290,13 +1053,13 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -1317,13 +1080,13 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1344,16 +1107,16 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -1374,16 +1137,16 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -1404,13 +1167,13 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -1431,13 +1194,13 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -1458,16 +1221,16 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -1488,13 +1251,13 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -1515,13 +1278,13 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -1542,16 +1305,16 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -1572,13 +1335,13 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -1599,16 +1362,16 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -1629,16 +1392,16 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -1659,13 +1422,13 @@
         <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -1686,13 +1449,13 @@
         <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -1713,13 +1476,13 @@
         <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -1740,16 +1503,16 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -1765,18 +1528,18 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31" s="3">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -1790,8 +1553,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J31" s="5" t="s">
-        <v>32</v>
+      <c r="J31" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1800,13 +1563,13 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -1827,13 +1590,13 @@
         <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -1854,13 +1617,13 @@
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
@@ -1881,13 +1644,13 @@
         <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -1908,13 +1671,13 @@
         <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
@@ -1935,13 +1698,13 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
@@ -1962,13 +1725,13 @@
         <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
@@ -1989,13 +1752,13 @@
         <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
@@ -2016,16 +1779,16 @@
         <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
@@ -2046,13 +1809,13 @@
         <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
@@ -2073,13 +1836,13 @@
         <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
@@ -2095,18 +1858,18 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+      <c r="A43" s="3">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
@@ -2127,13 +1890,13 @@
         <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
@@ -2154,13 +1917,13 @@
         <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
@@ -2181,13 +1944,13 @@
         <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
@@ -2208,13 +1971,13 @@
         <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
@@ -2230,18 +1993,18 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+      <c r="A48" s="3">
         <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
@@ -2257,18 +2020,18 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="6">
+      <c r="A49" s="4">
         <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G49">
         <f t="shared" si="0"/>
@@ -2289,13 +2052,13 @@
         <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G50">
         <f t="shared" si="0"/>
@@ -2316,13 +2079,13 @@
         <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G51">
         <f t="shared" si="0"/>
@@ -2343,13 +2106,13 @@
         <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G52">
         <f t="shared" si="0"/>
@@ -2370,13 +2133,13 @@
         <v>154</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G53">
         <f t="shared" si="0"/>
@@ -2397,13 +2160,13 @@
         <v>157</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G54">
         <f t="shared" si="0"/>
@@ -2424,13 +2187,13 @@
         <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G55">
         <f t="shared" si="0"/>
@@ -2451,16 +2214,16 @@
         <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G56">
         <f t="shared" si="0"/>
@@ -2481,13 +2244,13 @@
         <v>166</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G57">
         <f t="shared" si="0"/>
@@ -2503,18 +2266,18 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="5">
+      <c r="A58" s="3">
         <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G58">
         <f t="shared" si="0"/>
@@ -2528,8 +2291,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J58" s="5" t="s">
-        <v>33</v>
+      <c r="J58" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2538,13 +2301,13 @@
         <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G59">
         <f t="shared" si="0"/>
@@ -2565,13 +2328,13 @@
         <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G60">
         <f t="shared" si="0"/>
@@ -2592,13 +2355,13 @@
         <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G61">
         <f t="shared" si="0"/>
@@ -2619,13 +2382,13 @@
         <v>181</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G62">
         <f t="shared" si="0"/>
@@ -2646,13 +2409,13 @@
         <v>184</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G63">
         <f t="shared" si="0"/>
@@ -2673,13 +2436,13 @@
         <v>187</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G64">
         <f t="shared" si="0"/>
@@ -2728,7 +2491,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C70" s="2">
         <f>I65/A66</f>
@@ -2737,12 +2500,12 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C73" s="2">
         <f>C74*(C75*(1-C75)/C76)^(1/2)</f>
@@ -2751,7 +2514,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C74">
         <v>1.96</v>
@@ -2759,16 +2522,16 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" s="7">
+        <v>19</v>
+      </c>
+      <c r="C75" s="5">
         <f>C69</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C76">
         <f>A66</f>
@@ -2776,8 +2539,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="8" t="s">
-        <v>35</v>
+      <c r="A79" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2814,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2826,10 +2589,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -2843,16 +2606,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
@@ -2873,16 +2636,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:I52" si="0">IF(B3="si",1,0)</f>
@@ -2903,13 +2666,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2930,16 +2693,16 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -2960,16 +2723,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -2990,13 +2753,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -3017,16 +2780,16 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -3047,13 +2810,13 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -3074,13 +2837,13 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -3101,13 +2864,13 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -3128,13 +2891,13 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -3155,13 +2918,13 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -3182,13 +2945,13 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -3209,13 +2972,13 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -3236,13 +2999,13 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -3263,13 +3026,13 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -3290,13 +3053,13 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -3317,16 +3080,16 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -3347,13 +3110,13 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -3374,16 +3137,16 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -3404,13 +3167,13 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -3431,16 +3194,16 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -3461,16 +3224,16 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -3491,13 +3254,13 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -3518,13 +3281,13 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -3545,13 +3308,13 @@
         <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -3572,16 +3335,16 @@
         <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -3602,13 +3365,13 @@
         <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -3629,16 +3392,16 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -3659,13 +3422,13 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -3686,13 +3449,13 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -3713,13 +3476,13 @@
         <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -3740,13 +3503,13 @@
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
@@ -3767,13 +3530,13 @@
         <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -3794,13 +3557,13 @@
         <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
@@ -3821,16 +3584,16 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
@@ -3851,13 +3614,13 @@
         <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
@@ -3878,16 +3641,16 @@
         <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F39" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
@@ -3908,13 +3671,13 @@
         <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
@@ -3935,13 +3698,13 @@
         <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
@@ -3962,16 +3725,16 @@
         <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
@@ -3992,13 +3755,13 @@
         <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
@@ -4019,13 +3782,13 @@
         <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
@@ -4046,13 +3809,13 @@
         <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
@@ -4073,13 +3836,13 @@
         <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
@@ -4100,13 +3863,13 @@
         <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
@@ -4127,13 +3890,13 @@
         <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
@@ -4154,13 +3917,13 @@
         <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G49">
         <f t="shared" si="0"/>
@@ -4181,13 +3944,13 @@
         <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G50">
         <f t="shared" si="0"/>
@@ -4208,13 +3971,13 @@
         <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G51">
         <f t="shared" si="0"/>
@@ -4235,16 +3998,16 @@
         <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G52">
         <f t="shared" si="0"/>
@@ -4304,12 +4067,12 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C61" s="2">
         <f>C62*(C63*(1-C63)/C64)^(1/2)</f>
@@ -4318,7 +4081,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C62">
         <v>1.96</v>
@@ -4326,7 +4089,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C63" s="2">
         <f>C57</f>
@@ -4335,7 +4098,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C64">
         <f>A55</f>
@@ -4343,8 +4106,8 @@
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="8" t="s">
-        <v>36</v>
+      <c r="A67" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4361,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1FF2E0-CBF5-4429-A8E7-8C52D40AA9F4}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4381,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4393,10 +4156,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -4410,16 +4173,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <f>IF(B2="si",1,0)</f>
@@ -4440,13 +4203,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:I47" si="0">IF(B3="si",1,0)</f>
@@ -4467,13 +4230,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -4494,13 +4257,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -4521,13 +4284,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -4548,13 +4311,13 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -4575,16 +4338,16 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -4605,13 +4368,13 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -4632,16 +4395,16 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -4662,19 +4425,19 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -4695,16 +4458,16 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -4725,13 +4488,13 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -4752,16 +4515,16 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -4782,16 +4545,16 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -4812,13 +4575,13 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -4839,16 +4602,16 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -4869,13 +4632,13 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -4896,16 +4659,16 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -4926,13 +4689,13 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -4953,13 +4716,13 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -4980,16 +4743,16 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -5010,16 +4773,16 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -5040,16 +4803,16 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -5070,16 +4833,16 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -5100,13 +4863,13 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -5127,16 +4890,16 @@
         <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -5157,16 +4920,16 @@
         <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -5187,13 +4950,13 @@
         <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -5214,13 +4977,13 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -5241,13 +5004,13 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -5268,16 +5031,16 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -5298,13 +5061,13 @@
         <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -5325,13 +5088,13 @@
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
@@ -5352,16 +5115,16 @@
         <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -5381,17 +5144,29 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -5399,13 +5174,25 @@
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
@@ -5417,17 +5204,29 @@
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -5435,17 +5234,26 @@
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>24</v>
+      </c>
       <c r="G39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -5453,17 +5261,26 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
       <c r="G40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -5471,9 +5288,18 @@
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
       <c r="G41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
@@ -5489,13 +5315,25 @@
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
       <c r="G42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
@@ -5507,13 +5345,22 @@
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
       <c r="G43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
@@ -5525,9 +5372,18 @@
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>24</v>
+      </c>
       <c r="G44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
@@ -5535,7 +5391,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -5543,17 +5399,29 @@
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" t="s">
+        <v>24</v>
+      </c>
       <c r="G45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -5561,17 +5429,29 @@
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" t="s">
+        <v>24</v>
+      </c>
       <c r="G46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -5579,13 +5459,25 @@
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>24</v>
+      </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
@@ -5598,15 +5490,15 @@
       </c>
       <c r="G48">
         <f>SUM(G2:G47)</f>
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H48">
         <f>SUM(H2:H47)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I48">
         <f>SUM(I2:I47)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -5621,7 +5513,7 @@
       </c>
       <c r="C51" s="2">
         <f>H48/A49</f>
-        <v>0.63043478260869568</v>
+        <v>0.84782608695652173</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -5630,26 +5522,26 @@
       </c>
       <c r="C52" s="2">
         <f>I48/A49</f>
-        <v>0.43478260869565216</v>
+        <v>0.58695652173913049</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C55" s="2">
         <f>C56*(C57*(1-C57)/C58)^(1/2)</f>
-        <v>0</v>
+        <v>0.10380078725868275</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C56">
         <v>1.96</v>
@@ -5657,13 +5549,16 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C57" s="2">
+        <f>C51</f>
+        <v>0.84782608695652173</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <f>A49</f>
@@ -5671,8 +5566,8 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>37</v>
+      <c r="A61" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando cambios para incorporar mistral y lograr menos pérdidas de preguntas
</commit_message>
<xml_diff>
--- a/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
+++ b/docs/Analisis_de_resultados/analisis_22_05_25/Analisis_muestreo_22_05_25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\python_con_json\obtener_preguntas_y_respuestas\docs\Analisis_de_resultados\analisis_22_05_25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29462C60-E9AA-4153-8B18-7752CF729782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC208B0-D715-4805-BDDD-B18BF0E4188B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{6B6DCE76-2FEF-49B0-BD73-CEFB42CCE8FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Referencias" sheetId="5" r:id="rId1"/>
@@ -215,14 +215,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,90 +559,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AA836D-385C-4141-AF5A-AAFCA35CFBC3}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-    </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2558,7 +2551,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4124,7 +4117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1FF2E0-CBF5-4429-A8E7-8C52D40AA9F4}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -5566,7 +5559,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+      <c r="A61" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>